<commit_message>
hopefully last push before presentation
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyemin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamet\Dropbox (GaTech)\Summer 2018\CS 6795\Project2\CS6795-project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{278CD7DD-3B52-4688-A36D-E2269870FE7F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="6120" windowWidth="34860" windowHeight="18520" tabRatio="500"/>
+    <workbookView xWindow="7463" yWindow="6120" windowWidth="34860" windowHeight="18518" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -221,6 +222,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -488,16 +492,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,8 +620,62 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.5">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.5">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.5">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.5">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.5">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.5">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>